<commit_message>
15 Jan - Initial
</commit_message>
<xml_diff>
--- a/TestData/T1503_Contact_ContactDetails_AddEditDeleteActivity.xlsx
+++ b/TestData/T1503_Contact_ContactDetails_AddEditDeleteActivity.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoyal0630\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768C612-CEB5-46B0-BB7E-75F137D49F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9360" windowHeight="1950" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="ContactTypes" sheetId="4" r:id="rId3"/>
-    <sheet name="Users" sheetId="2" r:id="rId4"/>
-    <sheet name="Activity" sheetId="3" r:id="rId5"/>
+    <sheet name="ContactTypes" sheetId="4" r:id="rId2"/>
+    <sheet name="Users" sheetId="2" r:id="rId3"/>
+    <sheet name="Activity" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>CompanyName</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Houlihan Employee</t>
   </si>
   <si>
-    <t>StdUser</t>
-  </si>
-  <si>
     <t>ActivityType</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Houlihan</t>
   </si>
   <si>
-    <t>Ayati Arvind</t>
-  </si>
-  <si>
     <t>StandardTestCompany</t>
   </si>
   <si>
@@ -94,12 +88,24 @@
   </si>
   <si>
     <t>James</t>
+  </si>
+  <si>
+    <t>Test Meeting</t>
+  </si>
+  <si>
+    <t>Test Other</t>
+  </si>
+  <si>
+    <t>CF Financial</t>
+  </si>
+  <si>
+    <t>Thomas Bailey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,22 +425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,26 +451,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -473,41 +479,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -517,29 +511,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -547,52 +541,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial - 16th Jan 2025
</commit_message>
<xml_diff>
--- a/TestData/T1503_Contact_ContactDetails_AddEditDeleteActivity.xlsx
+++ b/TestData/T1503_Contact_ContactDetails_AddEditDeleteActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768C612-CEB5-46B0-BB7E-75F137D49F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5979F6-DA9C-4B31-824B-61F9C22A18F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="1500" windowWidth="19416" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,16 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>ContactTypesValue</t>
   </si>
@@ -48,9 +39,6 @@
     <t>Houlihan Employee</t>
   </si>
   <si>
-    <t>ActivityType</t>
-  </si>
-  <si>
     <t>Call</t>
   </si>
   <si>
@@ -66,40 +54,97 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Test Activity</t>
-  </si>
-  <si>
-    <t>Test Subject</t>
-  </si>
-  <si>
-    <t>Houlihan</t>
-  </si>
-  <si>
     <t>StandardTestCompany</t>
   </si>
   <si>
-    <t>Sonika</t>
-  </si>
-  <si>
-    <t>Goyal</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Test Meeting</t>
-  </si>
-  <si>
-    <t>Test Other</t>
-  </si>
-  <si>
     <t>CF Financial</t>
   </si>
   <si>
     <t>Thomas Bailey</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>RelatedCompany</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Activity Test External Contact</t>
+  </si>
+  <si>
+    <t>ActivityCompany</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>IndustryGroup</t>
+  </si>
+  <si>
+    <t>ProductType</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>MeetingNotes</t>
+  </si>
+  <si>
+    <t>ExtAttendee</t>
+  </si>
+  <si>
+    <t>Automated Test Subject Meeting</t>
+  </si>
+  <si>
+    <t>BUS - Business Services</t>
+  </si>
+  <si>
+    <t>Activist Advisory</t>
+  </si>
+  <si>
+    <t>Automated Test Description Meeting</t>
+  </si>
+  <si>
+    <t>Meeting Notes 1</t>
+  </si>
+  <si>
+    <t>Test External</t>
+  </si>
+  <si>
+    <t>Automated Test Subject Call</t>
+  </si>
+  <si>
+    <t>Automated Test Description Call</t>
+  </si>
+  <si>
+    <t>Meeting Notes 2</t>
+  </si>
+  <si>
+    <t>Automated Test Subject Email</t>
+  </si>
+  <si>
+    <t>Automated Test Description Email</t>
+  </si>
+  <si>
+    <t>Meeting Notes 3</t>
+  </si>
+  <si>
+    <t>Automated Test Subject Other</t>
+  </si>
+  <si>
+    <t>Automated Test Description Other</t>
+  </si>
+  <si>
+    <t>Meeting Notes 4</t>
+  </si>
+  <si>
+    <t>Test Houlihan</t>
   </si>
 </sst>
 </file>
@@ -143,9 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,48 +477,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -493,17 +539,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -527,13 +573,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -543,56 +589,136 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mid - 16th Jan 2025
</commit_message>
<xml_diff>
--- a/TestData/T1503_Contact_ContactDetails_AddEditDeleteActivity.xlsx
+++ b/TestData/T1503_Contact_ContactDetails_AddEditDeleteActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5979F6-DA9C-4B31-824B-61F9C22A18F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D150FC9-1E18-4A8F-99F8-071BFE891736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="1500" windowWidth="19416" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1500" windowWidth="19416" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>ContactTypesValue</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>StandardTestCompany</t>
-  </si>
-  <si>
     <t>CF Financial</t>
   </si>
   <si>
@@ -144,7 +141,7 @@
     <t>Meeting Notes 4</t>
   </si>
   <si>
-    <t>Test Houlihan</t>
+    <t>HL</t>
   </si>
 </sst>
 </file>
@@ -477,7 +474,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,35 +485,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -573,13 +570,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -608,25 +605,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -634,22 +631,22 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -657,22 +654,22 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -680,22 +677,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -703,22 +700,22 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>